<commit_message>
- adding save test and asserting for comment
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/TryToLoad/CommentAsNoteWithNoTextBox.xlsx
+++ b/ClosedXML.Tests/Resource/TryToLoad/CommentAsNoteWithNoTextBox.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\closedxml\ClosedXML.Tests\Resource\TryToLoad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3183A13C-694C-48F4-8186-C743E11FD187}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF615C61-CC87-44A7-BBC1-86D017A8987D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Brandstetter, Roman</author>
+    <author>Autor</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{59CA7BE1-18ED-486F-8F48-7ED57A210780}">
@@ -40,7 +35,7 @@
             <rFont val="Segoe UI"/>
             <charset val="1"/>
           </rPr>
-          <t>Brandstetter, Roman:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -387,7 +382,7 @@
   <dimension ref="A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +390,7 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>